<commit_message>
Update LSA Data Dictionary FY2021.xlsx
Add Vet HH w/3+ Children (1336), CH HH 55+ (1534), and CH HH with 3+ Children (1536) to population list.
</commit_message>
<xml_diff>
--- a/LSA Data Dictionary FY2021.xlsx
+++ b/LSA Data Dictionary FY2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://squarepegdata-my.sharepoint.com/personal/molly_squarepegdata_com/Documents/GitHub/LSASampleCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="13_ncr:1_{83E998E8-FF1F-4227-897A-6FABEC67F4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4992FFE2-16BE-4CCB-9EE6-C1ACBBB01D98}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{83E998E8-FF1F-4227-897A-6FABEC67F4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5FDD97B-E9B2-4018-AE49-A30AB3815B49}"/>
   <bookViews>
-    <workbookView xWindow="-3810" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B02B7233-7B9E-4318-BE1B-2F97AB3B1B83}"/>
+    <workbookView xWindow="-3810" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B02B7233-7B9E-4318-BE1B-2F97AB3B1B83}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Columns!$A$1:$I$291</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Lists!$A$1:$D$629</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Lists!$A$1:$D$632</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3096" uniqueCount="1168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3102" uniqueCount="1171">
   <si>
     <t>File ID</t>
   </si>
@@ -3684,6 +3684,15 @@
   </si>
   <si>
     <t>Identifies ethnicity for head of household as reported in LSAPerson. (Note that although this uses the same list as LSAPerson.Ethnicity, the value cannot be -1 since -1 is never a valid value for a head of household.)</t>
+  </si>
+  <si>
+    <t>Veteran Household - 3+ Children</t>
+  </si>
+  <si>
+    <t>Chronically Homeless Household 55+</t>
+  </si>
+  <si>
+    <t>Chronically Homeless Household - 3+ Children</t>
   </si>
 </sst>
 </file>
@@ -4488,8 +4497,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J291"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="H78" sqref="H78"/>
     </sheetView>
@@ -12548,10 +12557,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B52880F-20AD-49BC-9FD8-A02C6FD116A7}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:XFC638"/>
+  <dimension ref="A1:XFC641"/>
   <sheetViews>
-    <sheetView topLeftCell="A616" workbookViewId="0">
-      <selection activeCell="A636" sqref="A636:B638"/>
+    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
+      <selection activeCell="D430" sqref="D430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26259,10 +26268,10 @@
       <c r="B394" t="s">
         <v>395</v>
       </c>
-      <c r="C394" s="44">
+      <c r="C394" s="46">
         <v>1334</v>
       </c>
-      <c r="D394" s="21" t="s">
+      <c r="D394" s="47" t="s">
         <v>498</v>
       </c>
     </row>
@@ -26273,11 +26282,11 @@
       <c r="B395" t="s">
         <v>395</v>
       </c>
-      <c r="C395" s="46">
-        <v>1415</v>
-      </c>
-      <c r="D395" s="47" t="s">
-        <v>1157</v>
+      <c r="C395" s="44">
+        <v>1336</v>
+      </c>
+      <c r="D395" s="21" t="s">
+        <v>1168</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.45">
@@ -26287,11 +26296,11 @@
       <c r="B396" t="s">
         <v>395</v>
       </c>
-      <c r="C396" s="44">
-        <v>1418</v>
-      </c>
-      <c r="D396" s="21" t="s">
-        <v>488</v>
+      <c r="C396" s="46">
+        <v>1415</v>
+      </c>
+      <c r="D396" s="47" t="s">
+        <v>1157</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.45">
@@ -26302,10 +26311,10 @@
         <v>395</v>
       </c>
       <c r="C397" s="44">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="D397" s="21" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.45">
@@ -26316,10 +26325,10 @@
         <v>395</v>
       </c>
       <c r="C398" s="44">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="D398" s="21" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.45">
@@ -26330,10 +26339,10 @@
         <v>395</v>
       </c>
       <c r="C399" s="44">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D399" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.45">
@@ -26344,10 +26353,10 @@
         <v>395</v>
       </c>
       <c r="C400" s="44">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="D400" s="21" t="s">
-        <v>581</v>
+        <v>491</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.45">
@@ -26358,10 +26367,10 @@
         <v>395</v>
       </c>
       <c r="C401" s="44">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="D401" s="21" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.45">
@@ -26372,10 +26381,10 @@
         <v>395</v>
       </c>
       <c r="C402" s="44">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="D402" s="21" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.45">
@@ -26386,10 +26395,10 @@
         <v>395</v>
       </c>
       <c r="C403" s="44">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="D403" s="21" t="s">
-        <v>1055</v>
+        <v>583</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.45">
@@ -26400,10 +26409,10 @@
         <v>395</v>
       </c>
       <c r="C404" s="44">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="D404" s="21" t="s">
-        <v>584</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.45">
@@ -26414,10 +26423,10 @@
         <v>395</v>
       </c>
       <c r="C405" s="44">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="D405" s="21" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.45">
@@ -26428,10 +26437,10 @@
         <v>395</v>
       </c>
       <c r="C406" s="44">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="D406" s="21" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.45">
@@ -26442,10 +26451,10 @@
         <v>395</v>
       </c>
       <c r="C407" s="44">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="D407" s="21" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.45">
@@ -26456,10 +26465,10 @@
         <v>395</v>
       </c>
       <c r="C408" s="44">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="D408" s="21" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.45">
@@ -26470,10 +26479,10 @@
         <v>395</v>
       </c>
       <c r="C409" s="44">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="D409" s="21" t="s">
-        <v>492</v>
+        <v>588</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.45">
@@ -26484,10 +26493,10 @@
         <v>395</v>
       </c>
       <c r="C410" s="44">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="D410" s="21" t="s">
-        <v>589</v>
+        <v>492</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.45">
@@ -26498,10 +26507,10 @@
         <v>395</v>
       </c>
       <c r="C411" s="44">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="D411" s="21" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.45">
@@ -26512,10 +26521,10 @@
         <v>395</v>
       </c>
       <c r="C412" s="44">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="D412" s="21" t="s">
-        <v>499</v>
+        <v>590</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.45">
@@ -26526,10 +26535,10 @@
         <v>395</v>
       </c>
       <c r="C413" s="44">
-        <v>1519</v>
+        <v>1434</v>
       </c>
       <c r="D413" s="21" t="s">
-        <v>620</v>
+        <v>499</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.45">
@@ -26540,10 +26549,10 @@
         <v>395</v>
       </c>
       <c r="C414" s="44">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="D414" s="21" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.45">
@@ -26554,10 +26563,10 @@
         <v>395</v>
       </c>
       <c r="C415" s="44">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="D415" s="21" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.45">
@@ -26568,10 +26577,10 @@
         <v>395</v>
       </c>
       <c r="C416" s="44">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="D416" s="21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.45">
@@ -26582,10 +26591,10 @@
         <v>395</v>
       </c>
       <c r="C417" s="44">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="D417" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.45">
@@ -26596,10 +26605,10 @@
         <v>395</v>
       </c>
       <c r="C418" s="44">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="D418" s="21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.45">
@@ -26610,10 +26619,10 @@
         <v>395</v>
       </c>
       <c r="C419" s="44">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="D419" s="21" t="s">
-        <v>1056</v>
+        <v>625</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.45">
@@ -26624,10 +26633,10 @@
         <v>395</v>
       </c>
       <c r="C420" s="44">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="D420" s="21" t="s">
-        <v>626</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.45">
@@ -26638,10 +26647,10 @@
         <v>395</v>
       </c>
       <c r="C421" s="44">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="D421" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.45">
@@ -26652,10 +26661,10 @@
         <v>395</v>
       </c>
       <c r="C422" s="44">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="D422" s="21" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.45">
@@ -26666,10 +26675,10 @@
         <v>395</v>
       </c>
       <c r="C423" s="44">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="D423" s="21" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.45">
@@ -26680,10 +26689,10 @@
         <v>395</v>
       </c>
       <c r="C424" s="44">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="D424" s="21" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.45">
@@ -26694,10 +26703,10 @@
         <v>395</v>
       </c>
       <c r="C425" s="44">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="D425" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.45">
@@ -26708,10 +26717,10 @@
         <v>395</v>
       </c>
       <c r="C426" s="44">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="D426" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.45">
@@ -26722,10 +26731,10 @@
         <v>395</v>
       </c>
       <c r="C427" s="44">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="D427" s="21" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.45">
@@ -26736,10 +26745,10 @@
         <v>395</v>
       </c>
       <c r="C428" s="44">
-        <v>5053</v>
+        <v>1533</v>
       </c>
       <c r="D428" s="21" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.45">
@@ -26749,11 +26758,11 @@
       <c r="B429" t="s">
         <v>395</v>
       </c>
-      <c r="C429" s="44">
-        <v>5054</v>
-      </c>
-      <c r="D429" s="21" t="s">
-        <v>636</v>
+      <c r="C429" s="46">
+        <v>1534</v>
+      </c>
+      <c r="D429" s="47" t="s">
+        <v>1169</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.45">
@@ -26763,11 +26772,11 @@
       <c r="B430" t="s">
         <v>395</v>
       </c>
-      <c r="C430" s="44">
-        <v>5055</v>
-      </c>
-      <c r="D430" s="21" t="s">
-        <v>504</v>
+      <c r="C430" s="46">
+        <v>1536</v>
+      </c>
+      <c r="D430" s="47" t="s">
+        <v>1170</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.45">
@@ -26778,10 +26787,10 @@
         <v>395</v>
       </c>
       <c r="C431" s="44">
-        <v>5056</v>
+        <v>5053</v>
       </c>
       <c r="D431" s="21" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.45">
@@ -26792,10 +26801,10 @@
         <v>395</v>
       </c>
       <c r="C432" s="44">
-        <v>5057</v>
+        <v>5054</v>
       </c>
       <c r="D432" s="21" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.45">
@@ -26806,10 +26815,10 @@
         <v>395</v>
       </c>
       <c r="C433" s="44">
-        <v>5058</v>
+        <v>5055</v>
       </c>
       <c r="D433" s="21" t="s">
-        <v>639</v>
+        <v>504</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.45">
@@ -26820,10 +26829,10 @@
         <v>395</v>
       </c>
       <c r="C434" s="44">
-        <v>5059</v>
+        <v>5056</v>
       </c>
       <c r="D434" s="21" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.45">
@@ -26834,10 +26843,10 @@
         <v>395</v>
       </c>
       <c r="C435" s="44">
-        <v>5060</v>
+        <v>5057</v>
       </c>
       <c r="D435" s="21" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.45">
@@ -26848,10 +26857,10 @@
         <v>395</v>
       </c>
       <c r="C436" s="44">
-        <v>5061</v>
+        <v>5058</v>
       </c>
       <c r="D436" s="21" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.45">
@@ -26862,10 +26871,10 @@
         <v>395</v>
       </c>
       <c r="C437" s="44">
-        <v>5062</v>
+        <v>5059</v>
       </c>
       <c r="D437" s="21" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.45">
@@ -26876,10 +26885,10 @@
         <v>395</v>
       </c>
       <c r="C438" s="44">
-        <v>5063</v>
+        <v>5060</v>
       </c>
       <c r="D438" s="21" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.45">
@@ -26890,10 +26899,10 @@
         <v>395</v>
       </c>
       <c r="C439" s="44">
-        <v>5064</v>
+        <v>5061</v>
       </c>
       <c r="D439" s="21" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.45">
@@ -26904,10 +26913,10 @@
         <v>395</v>
       </c>
       <c r="C440" s="44">
-        <v>5065</v>
+        <v>5062</v>
       </c>
       <c r="D440" s="21" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.45">
@@ -26918,10 +26927,10 @@
         <v>395</v>
       </c>
       <c r="C441" s="44">
-        <v>5066</v>
+        <v>5063</v>
       </c>
       <c r="D441" s="21" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.45">
@@ -26932,10 +26941,10 @@
         <v>395</v>
       </c>
       <c r="C442" s="44">
-        <v>5067</v>
+        <v>5064</v>
       </c>
       <c r="D442" s="21" t="s">
-        <v>500</v>
+        <v>645</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.45">
@@ -26946,10 +26955,10 @@
         <v>395</v>
       </c>
       <c r="C443" s="44">
-        <v>5068</v>
+        <v>5065</v>
       </c>
       <c r="D443" s="21" t="s">
-        <v>501</v>
+        <v>646</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.45">
@@ -26960,10 +26969,10 @@
         <v>395</v>
       </c>
       <c r="C444" s="44">
-        <v>5069</v>
+        <v>5066</v>
       </c>
       <c r="D444" s="21" t="s">
-        <v>502</v>
+        <v>647</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.45">
@@ -26974,10 +26983,10 @@
         <v>395</v>
       </c>
       <c r="C445" s="44">
-        <v>5070</v>
+        <v>5067</v>
       </c>
       <c r="D445" s="21" t="s">
-        <v>648</v>
+        <v>500</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.45">
@@ -26988,10 +26997,10 @@
         <v>395</v>
       </c>
       <c r="C446" s="44">
-        <v>5071</v>
+        <v>5068</v>
       </c>
       <c r="D446" s="21" t="s">
-        <v>649</v>
+        <v>501</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.45">
@@ -27002,10 +27011,10 @@
         <v>395</v>
       </c>
       <c r="C447" s="44">
-        <v>5153</v>
+        <v>5069</v>
       </c>
       <c r="D447" s="21" t="s">
-        <v>650</v>
+        <v>502</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.45">
@@ -27016,10 +27025,10 @@
         <v>395</v>
       </c>
       <c r="C448" s="44">
-        <v>5154</v>
+        <v>5070</v>
       </c>
       <c r="D448" s="21" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.45">
@@ -27030,10 +27039,10 @@
         <v>395</v>
       </c>
       <c r="C449" s="44">
-        <v>5155</v>
+        <v>5071</v>
       </c>
       <c r="D449" s="21" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.45">
@@ -27044,10 +27053,10 @@
         <v>395</v>
       </c>
       <c r="C450" s="44">
-        <v>5156</v>
+        <v>5153</v>
       </c>
       <c r="D450" s="21" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.45">
@@ -27058,10 +27067,10 @@
         <v>395</v>
       </c>
       <c r="C451" s="44">
-        <v>5157</v>
+        <v>5154</v>
       </c>
       <c r="D451" s="21" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.45">
@@ -27072,10 +27081,10 @@
         <v>395</v>
       </c>
       <c r="C452" s="44">
-        <v>5158</v>
+        <v>5155</v>
       </c>
       <c r="D452" s="21" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.45">
@@ -27086,10 +27095,10 @@
         <v>395</v>
       </c>
       <c r="C453" s="44">
-        <v>5159</v>
+        <v>5156</v>
       </c>
       <c r="D453" s="21" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.45">
@@ -27100,10 +27109,10 @@
         <v>395</v>
       </c>
       <c r="C454" s="44">
-        <v>5160</v>
+        <v>5157</v>
       </c>
       <c r="D454" s="21" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.45">
@@ -27114,10 +27123,10 @@
         <v>395</v>
       </c>
       <c r="C455" s="44">
-        <v>5161</v>
+        <v>5158</v>
       </c>
       <c r="D455" s="21" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.45">
@@ -27128,10 +27137,10 @@
         <v>395</v>
       </c>
       <c r="C456" s="44">
-        <v>5162</v>
+        <v>5159</v>
       </c>
       <c r="D456" s="21" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.45">
@@ -27142,10 +27151,10 @@
         <v>395</v>
       </c>
       <c r="C457" s="44">
-        <v>5163</v>
+        <v>5160</v>
       </c>
       <c r="D457" s="21" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.45">
@@ -27156,10 +27165,10 @@
         <v>395</v>
       </c>
       <c r="C458" s="44">
-        <v>5164</v>
+        <v>5161</v>
       </c>
       <c r="D458" s="21" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.45">
@@ -27170,10 +27179,10 @@
         <v>395</v>
       </c>
       <c r="C459" s="44">
-        <v>5165</v>
+        <v>5162</v>
       </c>
       <c r="D459" s="21" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.45">
@@ -27184,10 +27193,10 @@
         <v>395</v>
       </c>
       <c r="C460" s="44">
-        <v>5166</v>
+        <v>5163</v>
       </c>
       <c r="D460" s="21" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.45">
@@ -27198,10 +27207,10 @@
         <v>395</v>
       </c>
       <c r="C461" s="44">
-        <v>5167</v>
+        <v>5164</v>
       </c>
       <c r="D461" s="21" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.45">
@@ -27212,10 +27221,10 @@
         <v>395</v>
       </c>
       <c r="C462" s="44">
-        <v>5168</v>
+        <v>5165</v>
       </c>
       <c r="D462" s="21" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.45">
@@ -27226,10 +27235,10 @@
         <v>395</v>
       </c>
       <c r="C463" s="44">
-        <v>5169</v>
+        <v>5166</v>
       </c>
       <c r="D463" s="21" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.45">
@@ -27240,10 +27249,10 @@
         <v>395</v>
       </c>
       <c r="C464" s="44">
-        <v>5170</v>
+        <v>5167</v>
       </c>
       <c r="D464" s="21" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.45">
@@ -27254,10 +27263,10 @@
         <v>395</v>
       </c>
       <c r="C465" s="44">
-        <v>5171</v>
+        <v>5168</v>
       </c>
       <c r="D465" s="21" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.45">
@@ -27268,10 +27277,10 @@
         <v>395</v>
       </c>
       <c r="C466" s="44">
-        <v>5253</v>
+        <v>5169</v>
       </c>
       <c r="D466" s="21" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.45">
@@ -27282,10 +27291,10 @@
         <v>395</v>
       </c>
       <c r="C467" s="44">
-        <v>5254</v>
+        <v>5170</v>
       </c>
       <c r="D467" s="21" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.45">
@@ -27296,10 +27305,10 @@
         <v>395</v>
       </c>
       <c r="C468" s="44">
-        <v>5255</v>
+        <v>5171</v>
       </c>
       <c r="D468" s="21" t="s">
-        <v>509</v>
+        <v>668</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.45">
@@ -27310,10 +27319,10 @@
         <v>395</v>
       </c>
       <c r="C469" s="44">
-        <v>5256</v>
+        <v>5253</v>
       </c>
       <c r="D469" s="21" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.45">
@@ -27324,10 +27333,10 @@
         <v>395</v>
       </c>
       <c r="C470" s="44">
-        <v>5257</v>
+        <v>5254</v>
       </c>
       <c r="D470" s="21" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.45">
@@ -27338,10 +27347,10 @@
         <v>395</v>
       </c>
       <c r="C471" s="44">
-        <v>5258</v>
+        <v>5255</v>
       </c>
       <c r="D471" s="21" t="s">
-        <v>673</v>
+        <v>509</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.45">
@@ -27352,10 +27361,10 @@
         <v>395</v>
       </c>
       <c r="C472" s="44">
-        <v>5259</v>
+        <v>5256</v>
       </c>
       <c r="D472" s="21" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.45">
@@ -27366,10 +27375,10 @@
         <v>395</v>
       </c>
       <c r="C473" s="44">
-        <v>5260</v>
+        <v>5257</v>
       </c>
       <c r="D473" s="21" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.45">
@@ -27380,10 +27389,10 @@
         <v>395</v>
       </c>
       <c r="C474" s="44">
-        <v>5261</v>
+        <v>5258</v>
       </c>
       <c r="D474" s="21" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.45">
@@ -27394,10 +27403,10 @@
         <v>395</v>
       </c>
       <c r="C475" s="44">
-        <v>5262</v>
+        <v>5259</v>
       </c>
       <c r="D475" s="21" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.45">
@@ -27408,10 +27417,10 @@
         <v>395</v>
       </c>
       <c r="C476" s="44">
-        <v>5263</v>
+        <v>5260</v>
       </c>
       <c r="D476" s="21" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.45">
@@ -27422,10 +27431,10 @@
         <v>395</v>
       </c>
       <c r="C477" s="44">
-        <v>5264</v>
+        <v>5261</v>
       </c>
       <c r="D477" s="21" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.45">
@@ -27436,10 +27445,10 @@
         <v>395</v>
       </c>
       <c r="C478" s="44">
-        <v>5265</v>
+        <v>5262</v>
       </c>
       <c r="D478" s="21" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.45">
@@ -27450,10 +27459,10 @@
         <v>395</v>
       </c>
       <c r="C479" s="44">
-        <v>5266</v>
+        <v>5263</v>
       </c>
       <c r="D479" s="21" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.45">
@@ -27464,10 +27473,10 @@
         <v>395</v>
       </c>
       <c r="C480" s="44">
-        <v>5267</v>
+        <v>5264</v>
       </c>
       <c r="D480" s="21" t="s">
-        <v>505</v>
+        <v>679</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.45">
@@ -27478,10 +27487,10 @@
         <v>395</v>
       </c>
       <c r="C481" s="44">
-        <v>5268</v>
+        <v>5265</v>
       </c>
       <c r="D481" s="21" t="s">
-        <v>506</v>
+        <v>680</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.45">
@@ -27492,10 +27501,10 @@
         <v>395</v>
       </c>
       <c r="C482" s="44">
-        <v>5269</v>
+        <v>5266</v>
       </c>
       <c r="D482" s="21" t="s">
-        <v>507</v>
+        <v>681</v>
       </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.45">
@@ -27506,10 +27515,10 @@
         <v>395</v>
       </c>
       <c r="C483" s="44">
-        <v>5270</v>
+        <v>5267</v>
       </c>
       <c r="D483" s="21" t="s">
-        <v>682</v>
+        <v>505</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.45">
@@ -27520,52 +27529,52 @@
         <v>395</v>
       </c>
       <c r="C484" s="44">
-        <v>5271</v>
+        <v>5268</v>
       </c>
       <c r="D484" s="21" t="s">
-        <v>683</v>
+        <v>506</v>
       </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A485">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B485" t="s">
-        <v>398</v>
-      </c>
-      <c r="C485">
-        <v>1</v>
-      </c>
-      <c r="D485" t="s">
-        <v>684</v>
+        <v>395</v>
+      </c>
+      <c r="C485" s="44">
+        <v>5269</v>
+      </c>
+      <c r="D485" s="21" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A486">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B486" t="s">
-        <v>398</v>
-      </c>
-      <c r="C486">
-        <v>2</v>
-      </c>
-      <c r="D486" t="s">
-        <v>685</v>
+        <v>395</v>
+      </c>
+      <c r="C486" s="44">
+        <v>5270</v>
+      </c>
+      <c r="D486" s="21" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A487">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B487" t="s">
-        <v>398</v>
-      </c>
-      <c r="C487">
-        <v>3</v>
-      </c>
-      <c r="D487" t="s">
-        <v>686</v>
+        <v>395</v>
+      </c>
+      <c r="C487" s="44">
+        <v>5271</v>
+      </c>
+      <c r="D487" s="21" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.45">
@@ -27576,10 +27585,10 @@
         <v>398</v>
       </c>
       <c r="C488">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D488" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.45">
@@ -27590,10 +27599,10 @@
         <v>398</v>
       </c>
       <c r="C489">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D489" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.45">
@@ -27604,10 +27613,10 @@
         <v>398</v>
       </c>
       <c r="C490">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D490" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.45">
@@ -27618,10 +27627,10 @@
         <v>398</v>
       </c>
       <c r="C491">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D491" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.45">
@@ -27632,10 +27641,10 @@
         <v>398</v>
       </c>
       <c r="C492">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D492" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.45">
@@ -27646,10 +27655,10 @@
         <v>398</v>
       </c>
       <c r="C493">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D493" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.45">
@@ -27660,10 +27669,10 @@
         <v>398</v>
       </c>
       <c r="C494">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D494" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.45">
@@ -27674,10 +27683,10 @@
         <v>398</v>
       </c>
       <c r="C495">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D495" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.45">
@@ -27688,10 +27697,10 @@
         <v>398</v>
       </c>
       <c r="C496">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D496" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.45">
@@ -27702,10 +27711,10 @@
         <v>398</v>
       </c>
       <c r="C497">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D497" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.45">
@@ -27716,10 +27725,10 @@
         <v>398</v>
       </c>
       <c r="C498">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D498" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.45">
@@ -27730,10 +27739,10 @@
         <v>398</v>
       </c>
       <c r="C499">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D499" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.45">
@@ -27744,10 +27753,10 @@
         <v>398</v>
       </c>
       <c r="C500">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D500" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.45">
@@ -27758,10 +27767,10 @@
         <v>398</v>
       </c>
       <c r="C501">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D501" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.45">
@@ -27772,10 +27781,10 @@
         <v>398</v>
       </c>
       <c r="C502">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D502" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.45">
@@ -27786,10 +27795,10 @@
         <v>398</v>
       </c>
       <c r="C503">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D503" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.45">
@@ -27800,10 +27809,10 @@
         <v>398</v>
       </c>
       <c r="C504">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D504" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.45">
@@ -27814,10 +27823,10 @@
         <v>398</v>
       </c>
       <c r="C505">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D505" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.45">
@@ -27828,10 +27837,10 @@
         <v>398</v>
       </c>
       <c r="C506">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D506" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.45">
@@ -27842,10 +27851,10 @@
         <v>398</v>
       </c>
       <c r="C507">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D507" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.45">
@@ -27856,10 +27865,10 @@
         <v>398</v>
       </c>
       <c r="C508">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D508" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.45">
@@ -27870,10 +27879,10 @@
         <v>398</v>
       </c>
       <c r="C509">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D509" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.45">
@@ -27884,10 +27893,10 @@
         <v>398</v>
       </c>
       <c r="C510">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D510" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.45">
@@ -27898,10 +27907,10 @@
         <v>398</v>
       </c>
       <c r="C511">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D511" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.45">
@@ -27912,10 +27921,10 @@
         <v>398</v>
       </c>
       <c r="C512">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D512" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.45">
@@ -27926,10 +27935,10 @@
         <v>398</v>
       </c>
       <c r="C513">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D513" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="514" spans="1:4" x14ac:dyDescent="0.45">
@@ -27940,10 +27949,10 @@
         <v>398</v>
       </c>
       <c r="C514">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D514" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
     </row>
     <row r="515" spans="1:4" x14ac:dyDescent="0.45">
@@ -27954,10 +27963,10 @@
         <v>398</v>
       </c>
       <c r="C515">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D515" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
     </row>
     <row r="516" spans="1:4" x14ac:dyDescent="0.45">
@@ -27968,10 +27977,10 @@
         <v>398</v>
       </c>
       <c r="C516">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D516" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.45">
@@ -27982,10 +27991,10 @@
         <v>398</v>
       </c>
       <c r="C517">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D517" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.45">
@@ -27996,10 +28005,10 @@
         <v>398</v>
       </c>
       <c r="C518">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D518" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
     </row>
     <row r="519" spans="1:4" x14ac:dyDescent="0.45">
@@ -28010,10 +28019,10 @@
         <v>398</v>
       </c>
       <c r="C519">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D519" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="520" spans="1:4" x14ac:dyDescent="0.45">
@@ -28024,10 +28033,10 @@
         <v>398</v>
       </c>
       <c r="C520">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D520" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="521" spans="1:4" x14ac:dyDescent="0.45">
@@ -28038,10 +28047,10 @@
         <v>398</v>
       </c>
       <c r="C521">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D521" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="522" spans="1:4" x14ac:dyDescent="0.45">
@@ -28052,10 +28061,10 @@
         <v>398</v>
       </c>
       <c r="C522">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D522" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="523" spans="1:4" x14ac:dyDescent="0.45">
@@ -28066,10 +28075,10 @@
         <v>398</v>
       </c>
       <c r="C523">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D523" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.45">
@@ -28080,10 +28089,10 @@
         <v>398</v>
       </c>
       <c r="C524">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D524" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.45">
@@ -28094,10 +28103,10 @@
         <v>398</v>
       </c>
       <c r="C525">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D525" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.45">
@@ -28108,10 +28117,10 @@
         <v>398</v>
       </c>
       <c r="C526">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D526" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="527" spans="1:4" x14ac:dyDescent="0.45">
@@ -28122,10 +28131,10 @@
         <v>398</v>
       </c>
       <c r="C527">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D527" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.45">
@@ -28136,10 +28145,10 @@
         <v>398</v>
       </c>
       <c r="C528">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D528" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.45">
@@ -28150,10 +28159,10 @@
         <v>398</v>
       </c>
       <c r="C529">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D529" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.45">
@@ -28164,10 +28173,10 @@
         <v>398</v>
       </c>
       <c r="C530">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D530" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
     <row r="531" spans="1:4" x14ac:dyDescent="0.45">
@@ -28178,10 +28187,10 @@
         <v>398</v>
       </c>
       <c r="C531">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D531" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.45">
@@ -28192,10 +28201,10 @@
         <v>398</v>
       </c>
       <c r="C532">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D532" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.45">
@@ -28206,10 +28215,10 @@
         <v>398</v>
       </c>
       <c r="C533">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D533" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.45">
@@ -28220,10 +28229,10 @@
         <v>398</v>
       </c>
       <c r="C534">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D534" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.45">
@@ -28234,10 +28243,10 @@
         <v>398</v>
       </c>
       <c r="C535">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D535" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.45">
@@ -28248,10 +28257,10 @@
         <v>398</v>
       </c>
       <c r="C536">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D536" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.45">
@@ -28262,10 +28271,10 @@
         <v>398</v>
       </c>
       <c r="C537">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D537" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.45">
@@ -28276,10 +28285,10 @@
         <v>398</v>
       </c>
       <c r="C538">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D538" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.45">
@@ -28290,10 +28299,10 @@
         <v>398</v>
       </c>
       <c r="C539">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D539" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.45">
@@ -28304,10 +28313,10 @@
         <v>398</v>
       </c>
       <c r="C540">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D540" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.45">
@@ -28318,10 +28327,10 @@
         <v>398</v>
       </c>
       <c r="C541">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D541" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.45">
@@ -28332,10 +28341,10 @@
         <v>398</v>
       </c>
       <c r="C542">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D542" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="543" spans="1:4" x14ac:dyDescent="0.45">
@@ -28346,10 +28355,10 @@
         <v>398</v>
       </c>
       <c r="C543">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D543" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.45">
@@ -28360,10 +28369,10 @@
         <v>398</v>
       </c>
       <c r="C544">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D544" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="545" spans="1:4" x14ac:dyDescent="0.45">
@@ -28374,10 +28383,10 @@
         <v>398</v>
       </c>
       <c r="C545">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D545" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="546" spans="1:4" x14ac:dyDescent="0.45">
@@ -28388,10 +28397,10 @@
         <v>398</v>
       </c>
       <c r="C546">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D546" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.45">
@@ -28402,10 +28411,10 @@
         <v>398</v>
       </c>
       <c r="C547">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D547" t="s">
-        <v>1017</v>
+        <v>743</v>
       </c>
     </row>
     <row r="548" spans="1:4" x14ac:dyDescent="0.45">
@@ -28416,52 +28425,52 @@
         <v>398</v>
       </c>
       <c r="C548">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D548" t="s">
-        <v>1018</v>
+        <v>744</v>
       </c>
     </row>
     <row r="549" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A549">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B549" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="C549">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="D549" t="s">
-        <v>970</v>
+        <v>745</v>
       </c>
     </row>
     <row r="550" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A550">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B550" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="C550">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="D550" t="s">
-        <v>971</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="551" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A551">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B551" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="C551">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D551" t="s">
-        <v>885</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="552" spans="1:4" x14ac:dyDescent="0.45">
@@ -28472,10 +28481,10 @@
         <v>412</v>
       </c>
       <c r="C552">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D552" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="553" spans="1:4" x14ac:dyDescent="0.45">
@@ -28486,10 +28495,10 @@
         <v>412</v>
       </c>
       <c r="C553">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D553" t="s">
-        <v>1019</v>
+        <v>971</v>
       </c>
     </row>
     <row r="554" spans="1:4" x14ac:dyDescent="0.45">
@@ -28500,10 +28509,10 @@
         <v>412</v>
       </c>
       <c r="C554">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D554" t="s">
-        <v>1020</v>
+        <v>885</v>
       </c>
     </row>
     <row r="555" spans="1:4" x14ac:dyDescent="0.45">
@@ -28514,164 +28523,164 @@
         <v>412</v>
       </c>
       <c r="C555">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D555" t="s">
-        <v>1021</v>
+        <v>972</v>
       </c>
     </row>
     <row r="556" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A556">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B556" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C556">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D556" t="s">
-        <v>753</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="557" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A557">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B557" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C557">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D557" t="s">
-        <v>754</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="558" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A558">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B558" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C558">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D558" t="s">
-        <v>784</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="559" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A559">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B559" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C559">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D559" t="s">
-        <v>785</v>
+        <v>753</v>
       </c>
     </row>
     <row r="560" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A560">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B560" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C560">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D560" t="s">
-        <v>786</v>
+        <v>754</v>
       </c>
     </row>
     <row r="561" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A561">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B561" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C561">
         <v>1</v>
       </c>
       <c r="D561" t="s">
-        <v>750</v>
+        <v>784</v>
       </c>
     </row>
     <row r="562" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A562">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B562" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C562">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D562" t="s">
-        <v>751</v>
+        <v>785</v>
       </c>
     </row>
     <row r="563" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A563">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B563" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C563">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D563" t="s">
-        <v>752</v>
+        <v>786</v>
       </c>
     </row>
     <row r="564" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A564">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B564" t="s">
-        <v>21</v>
+        <v>413</v>
       </c>
       <c r="C564">
         <v>1</v>
       </c>
       <c r="D564" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
     </row>
     <row r="565" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A565">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B565" t="s">
-        <v>21</v>
+        <v>413</v>
       </c>
       <c r="C565">
         <v>2</v>
       </c>
       <c r="D565" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
     </row>
     <row r="566" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A566">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B566" t="s">
-        <v>21</v>
+        <v>413</v>
       </c>
       <c r="C566">
         <v>3</v>
       </c>
       <c r="D566" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
     </row>
     <row r="567" spans="1:4" x14ac:dyDescent="0.45">
@@ -28682,10 +28691,10 @@
         <v>21</v>
       </c>
       <c r="C567">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D567" t="s">
-        <v>1022</v>
+        <v>755</v>
       </c>
     </row>
     <row r="568" spans="1:4" x14ac:dyDescent="0.45">
@@ -28696,10 +28705,10 @@
         <v>21</v>
       </c>
       <c r="C568">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D568" t="s">
-        <v>1023</v>
+        <v>756</v>
       </c>
     </row>
     <row r="569" spans="1:4" x14ac:dyDescent="0.45">
@@ -28710,10 +28719,10 @@
         <v>21</v>
       </c>
       <c r="C569">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D569" t="s">
-        <v>1024</v>
+        <v>757</v>
       </c>
     </row>
     <row r="570" spans="1:4" x14ac:dyDescent="0.45">
@@ -28724,10 +28733,10 @@
         <v>21</v>
       </c>
       <c r="C570">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D570" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="571" spans="1:4" x14ac:dyDescent="0.45">
@@ -28738,10 +28747,10 @@
         <v>21</v>
       </c>
       <c r="C571">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D571" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="572" spans="1:4" x14ac:dyDescent="0.45">
@@ -28752,10 +28761,10 @@
         <v>21</v>
       </c>
       <c r="C572">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D572" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="573" spans="1:4" x14ac:dyDescent="0.45">
@@ -28766,10 +28775,10 @@
         <v>21</v>
       </c>
       <c r="C573">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D573" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="574" spans="1:4" x14ac:dyDescent="0.45">
@@ -28780,10 +28789,10 @@
         <v>21</v>
       </c>
       <c r="C574">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D574" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="575" spans="1:4" x14ac:dyDescent="0.45">
@@ -28794,10 +28803,10 @@
         <v>21</v>
       </c>
       <c r="C575">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D575" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="576" spans="1:4" x14ac:dyDescent="0.45">
@@ -28808,10 +28817,10 @@
         <v>21</v>
       </c>
       <c r="C576">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D576" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="577" spans="1:4" x14ac:dyDescent="0.45">
@@ -28822,10 +28831,10 @@
         <v>21</v>
       </c>
       <c r="C577">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D577" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="578" spans="1:4" x14ac:dyDescent="0.45">
@@ -28836,10 +28845,10 @@
         <v>21</v>
       </c>
       <c r="C578">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D578" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="579" spans="1:4" x14ac:dyDescent="0.45">
@@ -28850,10 +28859,10 @@
         <v>21</v>
       </c>
       <c r="C579">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D579" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="580" spans="1:4" x14ac:dyDescent="0.45">
@@ -28864,10 +28873,10 @@
         <v>21</v>
       </c>
       <c r="C580">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D580" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="581" spans="1:4" x14ac:dyDescent="0.45">
@@ -28878,10 +28887,10 @@
         <v>21</v>
       </c>
       <c r="C581">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D581" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="582" spans="1:4" x14ac:dyDescent="0.45">
@@ -28892,10 +28901,10 @@
         <v>21</v>
       </c>
       <c r="C582">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D582" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="583" spans="1:4" x14ac:dyDescent="0.45">
@@ -28906,10 +28915,10 @@
         <v>21</v>
       </c>
       <c r="C583">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D583" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="584" spans="1:4" x14ac:dyDescent="0.45">
@@ -28920,10 +28929,10 @@
         <v>21</v>
       </c>
       <c r="C584">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D584" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="585" spans="1:4" x14ac:dyDescent="0.45">
@@ -28934,10 +28943,10 @@
         <v>21</v>
       </c>
       <c r="C585">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D585" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="586" spans="1:4" x14ac:dyDescent="0.45">
@@ -28948,10 +28957,10 @@
         <v>21</v>
       </c>
       <c r="C586">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D586" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="587" spans="1:4" x14ac:dyDescent="0.45">
@@ -28962,10 +28971,10 @@
         <v>21</v>
       </c>
       <c r="C587">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D587" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="588" spans="1:4" x14ac:dyDescent="0.45">
@@ -28976,10 +28985,10 @@
         <v>21</v>
       </c>
       <c r="C588">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D588" t="s">
-        <v>758</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="589" spans="1:4" x14ac:dyDescent="0.45">
@@ -28990,10 +28999,10 @@
         <v>21</v>
       </c>
       <c r="C589">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D589" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="590" spans="1:4" x14ac:dyDescent="0.45">
@@ -29004,10 +29013,10 @@
         <v>21</v>
       </c>
       <c r="C590">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D590" t="s">
-        <v>759</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="591" spans="1:4" x14ac:dyDescent="0.45">
@@ -29018,10 +29027,10 @@
         <v>21</v>
       </c>
       <c r="C591">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D591" t="s">
-        <v>1044</v>
+        <v>758</v>
       </c>
     </row>
     <row r="592" spans="1:4" x14ac:dyDescent="0.45">
@@ -29032,10 +29041,10 @@
         <v>21</v>
       </c>
       <c r="C592">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D592" t="s">
-        <v>760</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="593" spans="1:4" x14ac:dyDescent="0.45">
@@ -29046,10 +29055,10 @@
         <v>21</v>
       </c>
       <c r="C593">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D593" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="594" spans="1:4" x14ac:dyDescent="0.45">
@@ -29060,10 +29069,10 @@
         <v>21</v>
       </c>
       <c r="C594">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D594" t="s">
-        <v>786</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="595" spans="1:4" x14ac:dyDescent="0.45">
@@ -29074,10 +29083,10 @@
         <v>21</v>
       </c>
       <c r="C595">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D595" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="596" spans="1:4" x14ac:dyDescent="0.45">
@@ -29088,10 +29097,10 @@
         <v>21</v>
       </c>
       <c r="C596">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D596" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="597" spans="1:4" x14ac:dyDescent="0.45">
@@ -29102,10 +29111,10 @@
         <v>21</v>
       </c>
       <c r="C597">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D597" t="s">
-        <v>764</v>
+        <v>786</v>
       </c>
     </row>
     <row r="598" spans="1:4" x14ac:dyDescent="0.45">
@@ -29116,10 +29125,10 @@
         <v>21</v>
       </c>
       <c r="C598">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D598" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="599" spans="1:4" x14ac:dyDescent="0.45">
@@ -29130,10 +29139,10 @@
         <v>21</v>
       </c>
       <c r="C599">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D599" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
     </row>
     <row r="600" spans="1:4" x14ac:dyDescent="0.45">
@@ -29144,10 +29153,10 @@
         <v>21</v>
       </c>
       <c r="C600">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D600" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="601" spans="1:4" x14ac:dyDescent="0.45">
@@ -29158,10 +29167,10 @@
         <v>21</v>
       </c>
       <c r="C601">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D601" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="602" spans="1:4" x14ac:dyDescent="0.45">
@@ -29172,10 +29181,10 @@
         <v>21</v>
       </c>
       <c r="C602">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D602" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="603" spans="1:4" x14ac:dyDescent="0.45">
@@ -29186,10 +29195,10 @@
         <v>21</v>
       </c>
       <c r="C603">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D603" t="s">
-        <v>1045</v>
+        <v>767</v>
       </c>
     </row>
     <row r="604" spans="1:4" x14ac:dyDescent="0.45">
@@ -29200,10 +29209,10 @@
         <v>21</v>
       </c>
       <c r="C604">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D604" t="s">
-        <v>1046</v>
+        <v>768</v>
       </c>
     </row>
     <row r="605" spans="1:4" x14ac:dyDescent="0.45">
@@ -29214,10 +29223,10 @@
         <v>21</v>
       </c>
       <c r="C605">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D605" t="s">
-        <v>1047</v>
+        <v>769</v>
       </c>
     </row>
     <row r="606" spans="1:4" x14ac:dyDescent="0.45">
@@ -29228,80 +29237,80 @@
         <v>21</v>
       </c>
       <c r="C606">
+        <v>43</v>
+      </c>
+      <c r="D606" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="607" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A607">
+        <v>38</v>
+      </c>
+      <c r="B607" t="s">
+        <v>21</v>
+      </c>
+      <c r="C607">
+        <v>44</v>
+      </c>
+      <c r="D607" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="608" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A608">
+        <v>38</v>
+      </c>
+      <c r="B608" t="s">
+        <v>21</v>
+      </c>
+      <c r="C608">
+        <v>45</v>
+      </c>
+      <c r="D608" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="609" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A609">
+        <v>38</v>
+      </c>
+      <c r="B609" t="s">
+        <v>21</v>
+      </c>
+      <c r="C609">
         <v>46</v>
       </c>
-      <c r="D606" t="s">
+      <c r="D609" t="s">
         <v>1048</v>
-      </c>
-    </row>
-    <row r="607" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A607" s="22">
-        <v>38</v>
-      </c>
-      <c r="B607" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C607" s="22">
-        <v>47</v>
-      </c>
-      <c r="D607" s="22" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="608" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A608" s="22">
-        <v>38</v>
-      </c>
-      <c r="B608" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C608" s="22">
-        <v>48</v>
-      </c>
-      <c r="D608" s="22" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="609" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A609" s="22">
-        <v>38</v>
-      </c>
-      <c r="B609" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C609" s="21">
-        <v>49</v>
-      </c>
-      <c r="D609" s="21" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="610" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A610" s="22">
         <v>38</v>
       </c>
-      <c r="B610" s="21" t="s">
+      <c r="B610" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C610" s="21">
-        <v>50</v>
-      </c>
-      <c r="D610" s="21" t="s">
-        <v>771</v>
+      <c r="C610" s="22">
+        <v>47</v>
+      </c>
+      <c r="D610" s="22" t="s">
+        <v>1049</v>
       </c>
     </row>
     <row r="611" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A611" s="22">
         <v>38</v>
       </c>
-      <c r="B611" s="21" t="s">
+      <c r="B611" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C611" s="21">
-        <v>51</v>
-      </c>
-      <c r="D611" s="21" t="s">
-        <v>772</v>
+      <c r="C611" s="22">
+        <v>48</v>
+      </c>
+      <c r="D611" s="22" t="s">
+        <v>1050</v>
       </c>
     </row>
     <row r="612" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
@@ -29312,178 +29321,178 @@
         <v>21</v>
       </c>
       <c r="C612" s="21">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D612" s="21" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="613" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A613" s="22">
+        <v>38</v>
+      </c>
+      <c r="B613" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C613" s="21">
+        <v>50</v>
+      </c>
+      <c r="D613" s="21" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="614" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A614" s="22">
+        <v>38</v>
+      </c>
+      <c r="B614" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C614" s="21">
+        <v>51</v>
+      </c>
+      <c r="D614" s="21" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="615" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A615" s="22">
+        <v>38</v>
+      </c>
+      <c r="B615" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C615" s="21">
+        <v>52</v>
+      </c>
+      <c r="D615" s="21" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="616" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A616" s="22">
         <v>39</v>
       </c>
-      <c r="B613" s="22" t="s">
+      <c r="B616" s="22" t="s">
         <v>774</v>
       </c>
-      <c r="C613" s="22">
+      <c r="C616" s="22">
         <v>1</v>
       </c>
-      <c r="D613" s="22" t="s">
+      <c r="D616" s="22" t="s">
         <v>775</v>
-      </c>
-    </row>
-    <row r="614" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A614">
-        <v>39</v>
-      </c>
-      <c r="B614" t="s">
-        <v>774</v>
-      </c>
-      <c r="C614">
-        <v>3</v>
-      </c>
-      <c r="D614" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="615" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A615">
-        <v>39</v>
-      </c>
-      <c r="B615" t="s">
-        <v>774</v>
-      </c>
-      <c r="C615">
-        <v>4</v>
-      </c>
-      <c r="D615" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="616" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A616">
-        <v>40</v>
-      </c>
-      <c r="B616" t="s">
-        <v>435</v>
-      </c>
-      <c r="C616">
-        <v>1</v>
-      </c>
-      <c r="D616" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="617" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A617">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B617" t="s">
-        <v>435</v>
+        <v>774</v>
       </c>
       <c r="C617">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D617" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
     </row>
     <row r="618" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A618">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B618" t="s">
-        <v>435</v>
+        <v>774</v>
       </c>
       <c r="C618">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D618" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
     </row>
     <row r="619" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A619">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B619" t="s">
-        <v>778</v>
+        <v>435</v>
       </c>
       <c r="C619">
         <v>1</v>
       </c>
       <c r="D619" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
     </row>
     <row r="620" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A620">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B620" t="s">
-        <v>778</v>
+        <v>435</v>
       </c>
       <c r="C620">
         <v>2</v>
       </c>
       <c r="D620" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
     </row>
     <row r="621" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A621">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B621" t="s">
-        <v>778</v>
+        <v>435</v>
       </c>
       <c r="C621">
         <v>3</v>
       </c>
       <c r="D621" t="s">
-        <v>749</v>
+        <v>783</v>
       </c>
     </row>
     <row r="622" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A622">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B622" t="s">
-        <v>432</v>
+        <v>778</v>
       </c>
       <c r="C622">
         <v>1</v>
       </c>
       <c r="D622" t="s">
-        <v>788</v>
+        <v>779</v>
       </c>
     </row>
     <row r="623" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A623">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B623" t="s">
-        <v>432</v>
+        <v>778</v>
       </c>
       <c r="C623">
         <v>2</v>
       </c>
       <c r="D623" t="s">
-        <v>789</v>
+        <v>780</v>
       </c>
     </row>
     <row r="624" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A624">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B624" t="s">
-        <v>432</v>
+        <v>778</v>
       </c>
       <c r="C624">
         <v>3</v>
       </c>
       <c r="D624" t="s">
-        <v>790</v>
+        <v>749</v>
       </c>
     </row>
     <row r="625" spans="1:4" x14ac:dyDescent="0.45">
@@ -29494,52 +29503,52 @@
         <v>432</v>
       </c>
       <c r="C625">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="D625" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="626" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A626">
-        <v>43</v>
-      </c>
-      <c r="B626" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="C626" s="21">
-        <v>0</v>
-      </c>
-      <c r="D626" s="21" t="s">
-        <v>747</v>
+        <v>42</v>
+      </c>
+      <c r="B626" t="s">
+        <v>432</v>
+      </c>
+      <c r="C626">
+        <v>2</v>
+      </c>
+      <c r="D626" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="627" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A627">
-        <v>43</v>
-      </c>
-      <c r="B627" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="C627" s="21">
-        <v>1</v>
-      </c>
-      <c r="D627" s="21" t="s">
-        <v>1057</v>
+        <v>42</v>
+      </c>
+      <c r="B627" t="s">
+        <v>432</v>
+      </c>
+      <c r="C627">
+        <v>3</v>
+      </c>
+      <c r="D627" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="628" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A628">
-        <v>43</v>
-      </c>
-      <c r="B628" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="C628" s="21">
-        <v>2</v>
-      </c>
-      <c r="D628" s="21" t="s">
-        <v>1066</v>
+        <v>42</v>
+      </c>
+      <c r="B628" t="s">
+        <v>432</v>
+      </c>
+      <c r="C628">
+        <v>99</v>
+      </c>
+      <c r="D628" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="629" spans="1:4" x14ac:dyDescent="0.45">
@@ -29550,60 +29559,60 @@
         <v>152</v>
       </c>
       <c r="C629" s="21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D629" s="21" t="s">
-        <v>1067</v>
+        <v>747</v>
       </c>
     </row>
     <row r="630" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A630">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B630" s="21" t="s">
-        <v>1136</v>
+        <v>152</v>
       </c>
       <c r="C630" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D630" s="21" t="s">
-        <v>747</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="631" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A631">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B631" s="21" t="s">
-        <v>1136</v>
+        <v>152</v>
       </c>
       <c r="C631" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D631" s="21" t="s">
-        <v>748</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="632" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A632" s="45">
-        <v>44</v>
-      </c>
-      <c r="B632" s="45" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C632" s="45">
-        <v>-1</v>
-      </c>
-      <c r="D632" s="45" t="s">
-        <v>786</v>
+      <c r="A632">
+        <v>43</v>
+      </c>
+      <c r="B632" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C632" s="21">
+        <v>3</v>
+      </c>
+      <c r="D632" s="21" t="s">
+        <v>1067</v>
       </c>
     </row>
     <row r="633" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A633">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B633" s="21" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="C633" s="21">
         <v>0</v>
@@ -29614,10 +29623,10 @@
     </row>
     <row r="634" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A634">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B634" s="21" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="C634" s="21">
         <v>1</v>
@@ -29627,63 +29636,105 @@
       </c>
     </row>
     <row r="635" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A635">
-        <v>45</v>
-      </c>
-      <c r="B635" s="21" t="s">
-        <v>1138</v>
-      </c>
-      <c r="C635" s="21">
-        <v>2</v>
-      </c>
-      <c r="D635" s="21" t="s">
-        <v>1139</v>
+      <c r="A635" s="45">
+        <v>44</v>
+      </c>
+      <c r="B635" s="45" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C635" s="45">
+        <v>-1</v>
+      </c>
+      <c r="D635" s="45" t="s">
+        <v>786</v>
       </c>
     </row>
     <row r="636" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A636">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B636" s="21" t="s">
-        <v>281</v>
+        <v>1138</v>
       </c>
       <c r="C636" s="21">
         <v>0</v>
       </c>
       <c r="D636" s="21" t="s">
-        <v>1162</v>
+        <v>747</v>
       </c>
     </row>
     <row r="637" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A637">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B637" s="21" t="s">
-        <v>281</v>
+        <v>1138</v>
       </c>
       <c r="C637" s="21">
         <v>1</v>
       </c>
       <c r="D637" s="21" t="s">
-        <v>1163</v>
+        <v>748</v>
       </c>
     </row>
     <row r="638" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A638">
+        <v>45</v>
+      </c>
+      <c r="B638" s="21" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C638" s="21">
+        <v>2</v>
+      </c>
+      <c r="D638" s="21" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="639" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A639">
         <v>46</v>
       </c>
-      <c r="B638" s="21" t="s">
+      <c r="B639" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="C638" s="21">
+      <c r="C639" s="21">
+        <v>0</v>
+      </c>
+      <c r="D639" s="21" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="640" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A640">
+        <v>46</v>
+      </c>
+      <c r="B640" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="C640" s="21">
+        <v>1</v>
+      </c>
+      <c r="D640" s="21" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="641" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A641">
+        <v>46</v>
+      </c>
+      <c r="B641" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="C641" s="21">
         <v>99</v>
       </c>
-      <c r="D638" s="21" t="s">
+      <c r="D641" s="21" t="s">
         <v>875</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D629" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:D632" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update LSA Data Dictionary
Add 1535 (CH Parenting Child Households) to Population list.  Closes #839
</commit_message>
<xml_diff>
--- a/LSA Data Dictionary FY2021.xlsx
+++ b/LSA Data Dictionary FY2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://squarepegdata-my.sharepoint.com/personal/molly_squarepegdata_com/Documents/GitHub/LSASampleCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="13_ncr:1_{83E998E8-FF1F-4227-897A-6FABEC67F4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99375053-B872-456E-B2BE-CC980E49FDAB}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="13_ncr:1_{83E998E8-FF1F-4227-897A-6FABEC67F4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BC1903F-7A75-433B-BB26-FC07EB1F8BB1}"/>
   <bookViews>
-    <workbookView xWindow="-3810" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B02B7233-7B9E-4318-BE1B-2F97AB3B1B83}"/>
+    <workbookView xWindow="-3810" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B02B7233-7B9E-4318-BE1B-2F97AB3B1B83}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Columns!$A$1:$I$291</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Lists!$A$1:$D$632</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Lists!$A$1:$D$633</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3136" uniqueCount="1171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3138" uniqueCount="1172">
   <si>
     <t>File ID</t>
   </si>
@@ -3693,6 +3693,9 @@
   </si>
   <si>
     <t>50-82, 1176, 1177, 1276, 1277, subpops 53-71 of pops 50-52</t>
+  </si>
+  <si>
+    <t>Chronically Homeless Household - Parenting Child</t>
   </si>
 </sst>
 </file>
@@ -12557,9 +12560,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B52880F-20AD-49BC-9FD8-A02C6FD116A7}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:XFC641"/>
+  <dimension ref="A1:XFC642"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
+      <selection activeCell="K426" sqref="K426"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -26771,10 +26776,10 @@
         <v>395</v>
       </c>
       <c r="C430" s="46">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="D430" s="47" t="s">
-        <v>1168</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.45">
@@ -26784,11 +26789,11 @@
       <c r="B431" t="s">
         <v>395</v>
       </c>
-      <c r="C431" s="44">
-        <v>5053</v>
-      </c>
-      <c r="D431" s="21" t="s">
-        <v>635</v>
+      <c r="C431" s="46">
+        <v>1536</v>
+      </c>
+      <c r="D431" s="47" t="s">
+        <v>1168</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.45">
@@ -26799,10 +26804,10 @@
         <v>395</v>
       </c>
       <c r="C432" s="44">
-        <v>5054</v>
+        <v>5053</v>
       </c>
       <c r="D432" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.45">
@@ -26813,10 +26818,10 @@
         <v>395</v>
       </c>
       <c r="C433" s="44">
-        <v>5055</v>
+        <v>5054</v>
       </c>
       <c r="D433" s="21" t="s">
-        <v>504</v>
+        <v>636</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.45">
@@ -26827,10 +26832,10 @@
         <v>395</v>
       </c>
       <c r="C434" s="44">
-        <v>5056</v>
+        <v>5055</v>
       </c>
       <c r="D434" s="21" t="s">
-        <v>637</v>
+        <v>504</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.45">
@@ -26841,10 +26846,10 @@
         <v>395</v>
       </c>
       <c r="C435" s="44">
-        <v>5057</v>
+        <v>5056</v>
       </c>
       <c r="D435" s="21" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.45">
@@ -26855,10 +26860,10 @@
         <v>395</v>
       </c>
       <c r="C436" s="44">
-        <v>5058</v>
+        <v>5057</v>
       </c>
       <c r="D436" s="21" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.45">
@@ -26869,10 +26874,10 @@
         <v>395</v>
       </c>
       <c r="C437" s="44">
-        <v>5059</v>
+        <v>5058</v>
       </c>
       <c r="D437" s="21" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.45">
@@ -26883,10 +26888,10 @@
         <v>395</v>
       </c>
       <c r="C438" s="44">
-        <v>5060</v>
+        <v>5059</v>
       </c>
       <c r="D438" s="21" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.45">
@@ -26897,10 +26902,10 @@
         <v>395</v>
       </c>
       <c r="C439" s="44">
-        <v>5061</v>
+        <v>5060</v>
       </c>
       <c r="D439" s="21" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.45">
@@ -26911,10 +26916,10 @@
         <v>395</v>
       </c>
       <c r="C440" s="44">
-        <v>5062</v>
+        <v>5061</v>
       </c>
       <c r="D440" s="21" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.45">
@@ -26925,10 +26930,10 @@
         <v>395</v>
       </c>
       <c r="C441" s="44">
-        <v>5063</v>
+        <v>5062</v>
       </c>
       <c r="D441" s="21" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.45">
@@ -26939,10 +26944,10 @@
         <v>395</v>
       </c>
       <c r="C442" s="44">
-        <v>5064</v>
+        <v>5063</v>
       </c>
       <c r="D442" s="21" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.45">
@@ -26953,10 +26958,10 @@
         <v>395</v>
       </c>
       <c r="C443" s="44">
-        <v>5065</v>
+        <v>5064</v>
       </c>
       <c r="D443" s="21" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.45">
@@ -26967,10 +26972,10 @@
         <v>395</v>
       </c>
       <c r="C444" s="44">
-        <v>5066</v>
+        <v>5065</v>
       </c>
       <c r="D444" s="21" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.45">
@@ -26981,10 +26986,10 @@
         <v>395</v>
       </c>
       <c r="C445" s="44">
-        <v>5067</v>
+        <v>5066</v>
       </c>
       <c r="D445" s="21" t="s">
-        <v>500</v>
+        <v>647</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.45">
@@ -26995,10 +27000,10 @@
         <v>395</v>
       </c>
       <c r="C446" s="44">
-        <v>5068</v>
+        <v>5067</v>
       </c>
       <c r="D446" s="21" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.45">
@@ -27009,10 +27014,10 @@
         <v>395</v>
       </c>
       <c r="C447" s="44">
-        <v>5069</v>
+        <v>5068</v>
       </c>
       <c r="D447" s="21" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.45">
@@ -27023,10 +27028,10 @@
         <v>395</v>
       </c>
       <c r="C448" s="44">
-        <v>5070</v>
+        <v>5069</v>
       </c>
       <c r="D448" s="21" t="s">
-        <v>648</v>
+        <v>502</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.45">
@@ -27037,10 +27042,10 @@
         <v>395</v>
       </c>
       <c r="C449" s="44">
-        <v>5071</v>
+        <v>5070</v>
       </c>
       <c r="D449" s="21" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.45">
@@ -27051,10 +27056,10 @@
         <v>395</v>
       </c>
       <c r="C450" s="44">
-        <v>5153</v>
+        <v>5071</v>
       </c>
       <c r="D450" s="21" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.45">
@@ -27065,10 +27070,10 @@
         <v>395</v>
       </c>
       <c r="C451" s="44">
-        <v>5154</v>
+        <v>5153</v>
       </c>
       <c r="D451" s="21" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.45">
@@ -27079,10 +27084,10 @@
         <v>395</v>
       </c>
       <c r="C452" s="44">
-        <v>5155</v>
+        <v>5154</v>
       </c>
       <c r="D452" s="21" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.45">
@@ -27093,10 +27098,10 @@
         <v>395</v>
       </c>
       <c r="C453" s="44">
-        <v>5156</v>
+        <v>5155</v>
       </c>
       <c r="D453" s="21" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.45">
@@ -27107,10 +27112,10 @@
         <v>395</v>
       </c>
       <c r="C454" s="44">
-        <v>5157</v>
+        <v>5156</v>
       </c>
       <c r="D454" s="21" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.45">
@@ -27121,10 +27126,10 @@
         <v>395</v>
       </c>
       <c r="C455" s="44">
-        <v>5158</v>
+        <v>5157</v>
       </c>
       <c r="D455" s="21" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.45">
@@ -27135,10 +27140,10 @@
         <v>395</v>
       </c>
       <c r="C456" s="44">
-        <v>5159</v>
+        <v>5158</v>
       </c>
       <c r="D456" s="21" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.45">
@@ -27149,10 +27154,10 @@
         <v>395</v>
       </c>
       <c r="C457" s="44">
-        <v>5160</v>
+        <v>5159</v>
       </c>
       <c r="D457" s="21" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.45">
@@ -27163,10 +27168,10 @@
         <v>395</v>
       </c>
       <c r="C458" s="44">
-        <v>5161</v>
+        <v>5160</v>
       </c>
       <c r="D458" s="21" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.45">
@@ -27177,10 +27182,10 @@
         <v>395</v>
       </c>
       <c r="C459" s="44">
-        <v>5162</v>
+        <v>5161</v>
       </c>
       <c r="D459" s="21" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.45">
@@ -27191,10 +27196,10 @@
         <v>395</v>
       </c>
       <c r="C460" s="44">
-        <v>5163</v>
+        <v>5162</v>
       </c>
       <c r="D460" s="21" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.45">
@@ -27205,10 +27210,10 @@
         <v>395</v>
       </c>
       <c r="C461" s="44">
-        <v>5164</v>
+        <v>5163</v>
       </c>
       <c r="D461" s="21" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.45">
@@ -27219,10 +27224,10 @@
         <v>395</v>
       </c>
       <c r="C462" s="44">
-        <v>5165</v>
+        <v>5164</v>
       </c>
       <c r="D462" s="21" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.45">
@@ -27233,10 +27238,10 @@
         <v>395</v>
       </c>
       <c r="C463" s="44">
-        <v>5166</v>
+        <v>5165</v>
       </c>
       <c r="D463" s="21" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.45">
@@ -27247,10 +27252,10 @@
         <v>395</v>
       </c>
       <c r="C464" s="44">
-        <v>5167</v>
+        <v>5166</v>
       </c>
       <c r="D464" s="21" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.45">
@@ -27261,10 +27266,10 @@
         <v>395</v>
       </c>
       <c r="C465" s="44">
-        <v>5168</v>
+        <v>5167</v>
       </c>
       <c r="D465" s="21" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.45">
@@ -27275,10 +27280,10 @@
         <v>395</v>
       </c>
       <c r="C466" s="44">
-        <v>5169</v>
+        <v>5168</v>
       </c>
       <c r="D466" s="21" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.45">
@@ -27289,10 +27294,10 @@
         <v>395</v>
       </c>
       <c r="C467" s="44">
-        <v>5170</v>
+        <v>5169</v>
       </c>
       <c r="D467" s="21" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.45">
@@ -27303,10 +27308,10 @@
         <v>395</v>
       </c>
       <c r="C468" s="44">
-        <v>5171</v>
+        <v>5170</v>
       </c>
       <c r="D468" s="21" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.45">
@@ -27317,10 +27322,10 @@
         <v>395</v>
       </c>
       <c r="C469" s="44">
-        <v>5253</v>
+        <v>5171</v>
       </c>
       <c r="D469" s="21" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.45">
@@ -27331,10 +27336,10 @@
         <v>395</v>
       </c>
       <c r="C470" s="44">
-        <v>5254</v>
+        <v>5253</v>
       </c>
       <c r="D470" s="21" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.45">
@@ -27345,10 +27350,10 @@
         <v>395</v>
       </c>
       <c r="C471" s="44">
-        <v>5255</v>
+        <v>5254</v>
       </c>
       <c r="D471" s="21" t="s">
-        <v>509</v>
+        <v>670</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.45">
@@ -27359,10 +27364,10 @@
         <v>395</v>
       </c>
       <c r="C472" s="44">
-        <v>5256</v>
+        <v>5255</v>
       </c>
       <c r="D472" s="21" t="s">
-        <v>671</v>
+        <v>509</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.45">
@@ -27373,10 +27378,10 @@
         <v>395</v>
       </c>
       <c r="C473" s="44">
-        <v>5257</v>
+        <v>5256</v>
       </c>
       <c r="D473" s="21" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.45">
@@ -27387,10 +27392,10 @@
         <v>395</v>
       </c>
       <c r="C474" s="44">
-        <v>5258</v>
+        <v>5257</v>
       </c>
       <c r="D474" s="21" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.45">
@@ -27401,10 +27406,10 @@
         <v>395</v>
       </c>
       <c r="C475" s="44">
-        <v>5259</v>
+        <v>5258</v>
       </c>
       <c r="D475" s="21" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.45">
@@ -27415,10 +27420,10 @@
         <v>395</v>
       </c>
       <c r="C476" s="44">
-        <v>5260</v>
+        <v>5259</v>
       </c>
       <c r="D476" s="21" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.45">
@@ -27429,10 +27434,10 @@
         <v>395</v>
       </c>
       <c r="C477" s="44">
-        <v>5261</v>
+        <v>5260</v>
       </c>
       <c r="D477" s="21" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.45">
@@ -27443,10 +27448,10 @@
         <v>395</v>
       </c>
       <c r="C478" s="44">
-        <v>5262</v>
+        <v>5261</v>
       </c>
       <c r="D478" s="21" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.45">
@@ -27457,10 +27462,10 @@
         <v>395</v>
       </c>
       <c r="C479" s="44">
-        <v>5263</v>
+        <v>5262</v>
       </c>
       <c r="D479" s="21" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.45">
@@ -27471,10 +27476,10 @@
         <v>395</v>
       </c>
       <c r="C480" s="44">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="D480" s="21" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.45">
@@ -27485,10 +27490,10 @@
         <v>395</v>
       </c>
       <c r="C481" s="44">
-        <v>5265</v>
+        <v>5264</v>
       </c>
       <c r="D481" s="21" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.45">
@@ -27499,10 +27504,10 @@
         <v>395</v>
       </c>
       <c r="C482" s="44">
-        <v>5266</v>
+        <v>5265</v>
       </c>
       <c r="D482" s="21" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.45">
@@ -27513,10 +27518,10 @@
         <v>395</v>
       </c>
       <c r="C483" s="44">
-        <v>5267</v>
+        <v>5266</v>
       </c>
       <c r="D483" s="21" t="s">
-        <v>505</v>
+        <v>681</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.45">
@@ -27527,10 +27532,10 @@
         <v>395</v>
       </c>
       <c r="C484" s="44">
-        <v>5268</v>
+        <v>5267</v>
       </c>
       <c r="D484" s="21" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.45">
@@ -27541,10 +27546,10 @@
         <v>395</v>
       </c>
       <c r="C485" s="44">
-        <v>5269</v>
+        <v>5268</v>
       </c>
       <c r="D485" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.45">
@@ -27555,10 +27560,10 @@
         <v>395</v>
       </c>
       <c r="C486" s="44">
-        <v>5270</v>
+        <v>5269</v>
       </c>
       <c r="D486" s="21" t="s">
-        <v>682</v>
+        <v>507</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.45">
@@ -27569,24 +27574,24 @@
         <v>395</v>
       </c>
       <c r="C487" s="44">
-        <v>5271</v>
+        <v>5270</v>
       </c>
       <c r="D487" s="21" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A488">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B488" t="s">
-        <v>398</v>
-      </c>
-      <c r="C488">
-        <v>1</v>
-      </c>
-      <c r="D488" t="s">
-        <v>684</v>
+        <v>395</v>
+      </c>
+      <c r="C488" s="44">
+        <v>5271</v>
+      </c>
+      <c r="D488" s="21" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.45">
@@ -27597,10 +27602,10 @@
         <v>398</v>
       </c>
       <c r="C489">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D489" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.45">
@@ -27611,10 +27616,10 @@
         <v>398</v>
       </c>
       <c r="C490">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D490" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.45">
@@ -27625,10 +27630,10 @@
         <v>398</v>
       </c>
       <c r="C491">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D491" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.45">
@@ -27639,10 +27644,10 @@
         <v>398</v>
       </c>
       <c r="C492">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D492" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.45">
@@ -27653,10 +27658,10 @@
         <v>398</v>
       </c>
       <c r="C493">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D493" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.45">
@@ -27667,10 +27672,10 @@
         <v>398</v>
       </c>
       <c r="C494">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D494" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.45">
@@ -27681,10 +27686,10 @@
         <v>398</v>
       </c>
       <c r="C495">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D495" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.45">
@@ -27695,10 +27700,10 @@
         <v>398</v>
       </c>
       <c r="C496">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D496" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.45">
@@ -27709,10 +27714,10 @@
         <v>398</v>
       </c>
       <c r="C497">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D497" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.45">
@@ -27723,10 +27728,10 @@
         <v>398</v>
       </c>
       <c r="C498">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D498" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.45">
@@ -27737,10 +27742,10 @@
         <v>398</v>
       </c>
       <c r="C499">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D499" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.45">
@@ -27751,10 +27756,10 @@
         <v>398</v>
       </c>
       <c r="C500">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D500" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.45">
@@ -27765,10 +27770,10 @@
         <v>398</v>
       </c>
       <c r="C501">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D501" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.45">
@@ -27779,10 +27784,10 @@
         <v>398</v>
       </c>
       <c r="C502">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D502" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.45">
@@ -27793,10 +27798,10 @@
         <v>398</v>
       </c>
       <c r="C503">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D503" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.45">
@@ -27807,10 +27812,10 @@
         <v>398</v>
       </c>
       <c r="C504">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D504" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.45">
@@ -27821,10 +27826,10 @@
         <v>398</v>
       </c>
       <c r="C505">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D505" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.45">
@@ -27835,10 +27840,10 @@
         <v>398</v>
       </c>
       <c r="C506">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D506" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.45">
@@ -27849,10 +27854,10 @@
         <v>398</v>
       </c>
       <c r="C507">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D507" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.45">
@@ -27863,10 +27868,10 @@
         <v>398</v>
       </c>
       <c r="C508">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D508" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.45">
@@ -27877,10 +27882,10 @@
         <v>398</v>
       </c>
       <c r="C509">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D509" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.45">
@@ -27891,10 +27896,10 @@
         <v>398</v>
       </c>
       <c r="C510">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D510" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.45">
@@ -27905,10 +27910,10 @@
         <v>398</v>
       </c>
       <c r="C511">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D511" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.45">
@@ -27919,10 +27924,10 @@
         <v>398</v>
       </c>
       <c r="C512">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D512" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.45">
@@ -27933,10 +27938,10 @@
         <v>398</v>
       </c>
       <c r="C513">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D513" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="514" spans="1:4" x14ac:dyDescent="0.45">
@@ -27947,10 +27952,10 @@
         <v>398</v>
       </c>
       <c r="C514">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D514" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="515" spans="1:4" x14ac:dyDescent="0.45">
@@ -27961,10 +27966,10 @@
         <v>398</v>
       </c>
       <c r="C515">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D515" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="516" spans="1:4" x14ac:dyDescent="0.45">
@@ -27975,10 +27980,10 @@
         <v>398</v>
       </c>
       <c r="C516">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D516" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.45">
@@ -27989,10 +27994,10 @@
         <v>398</v>
       </c>
       <c r="C517">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D517" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.45">
@@ -28003,10 +28008,10 @@
         <v>398</v>
       </c>
       <c r="C518">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D518" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="519" spans="1:4" x14ac:dyDescent="0.45">
@@ -28017,10 +28022,10 @@
         <v>398</v>
       </c>
       <c r="C519">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D519" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="520" spans="1:4" x14ac:dyDescent="0.45">
@@ -28031,10 +28036,10 @@
         <v>398</v>
       </c>
       <c r="C520">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D520" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="521" spans="1:4" x14ac:dyDescent="0.45">
@@ -28045,10 +28050,10 @@
         <v>398</v>
       </c>
       <c r="C521">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D521" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="522" spans="1:4" x14ac:dyDescent="0.45">
@@ -28059,10 +28064,10 @@
         <v>398</v>
       </c>
       <c r="C522">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D522" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="523" spans="1:4" x14ac:dyDescent="0.45">
@@ -28073,10 +28078,10 @@
         <v>398</v>
       </c>
       <c r="C523">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D523" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.45">
@@ -28087,10 +28092,10 @@
         <v>398</v>
       </c>
       <c r="C524">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D524" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.45">
@@ -28101,10 +28106,10 @@
         <v>398</v>
       </c>
       <c r="C525">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D525" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.45">
@@ -28115,10 +28120,10 @@
         <v>398</v>
       </c>
       <c r="C526">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D526" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="527" spans="1:4" x14ac:dyDescent="0.45">
@@ -28129,10 +28134,10 @@
         <v>398</v>
       </c>
       <c r="C527">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D527" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.45">
@@ -28143,10 +28148,10 @@
         <v>398</v>
       </c>
       <c r="C528">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D528" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.45">
@@ -28157,10 +28162,10 @@
         <v>398</v>
       </c>
       <c r="C529">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D529" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.45">
@@ -28171,10 +28176,10 @@
         <v>398</v>
       </c>
       <c r="C530">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D530" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="531" spans="1:4" x14ac:dyDescent="0.45">
@@ -28185,10 +28190,10 @@
         <v>398</v>
       </c>
       <c r="C531">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D531" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.45">
@@ -28199,10 +28204,10 @@
         <v>398</v>
       </c>
       <c r="C532">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D532" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.45">
@@ -28213,10 +28218,10 @@
         <v>398</v>
       </c>
       <c r="C533">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D533" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.45">
@@ -28227,10 +28232,10 @@
         <v>398</v>
       </c>
       <c r="C534">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D534" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.45">
@@ -28241,10 +28246,10 @@
         <v>398</v>
       </c>
       <c r="C535">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D535" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.45">
@@ -28255,10 +28260,10 @@
         <v>398</v>
       </c>
       <c r="C536">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D536" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.45">
@@ -28269,10 +28274,10 @@
         <v>398</v>
       </c>
       <c r="C537">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D537" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.45">
@@ -28283,10 +28288,10 @@
         <v>398</v>
       </c>
       <c r="C538">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D538" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.45">
@@ -28297,10 +28302,10 @@
         <v>398</v>
       </c>
       <c r="C539">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D539" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.45">
@@ -28311,10 +28316,10 @@
         <v>398</v>
       </c>
       <c r="C540">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D540" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.45">
@@ -28325,10 +28330,10 @@
         <v>398</v>
       </c>
       <c r="C541">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D541" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.45">
@@ -28339,10 +28344,10 @@
         <v>398</v>
       </c>
       <c r="C542">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D542" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="543" spans="1:4" x14ac:dyDescent="0.45">
@@ -28353,10 +28358,10 @@
         <v>398</v>
       </c>
       <c r="C543">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D543" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.45">
@@ -28367,10 +28372,10 @@
         <v>398</v>
       </c>
       <c r="C544">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D544" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="545" spans="1:4" x14ac:dyDescent="0.45">
@@ -28381,10 +28386,10 @@
         <v>398</v>
       </c>
       <c r="C545">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D545" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="546" spans="1:4" x14ac:dyDescent="0.45">
@@ -28395,10 +28400,10 @@
         <v>398</v>
       </c>
       <c r="C546">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D546" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.45">
@@ -28409,10 +28414,10 @@
         <v>398</v>
       </c>
       <c r="C547">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D547" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="548" spans="1:4" x14ac:dyDescent="0.45">
@@ -28423,10 +28428,10 @@
         <v>398</v>
       </c>
       <c r="C548">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D548" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="549" spans="1:4" x14ac:dyDescent="0.45">
@@ -28437,10 +28442,10 @@
         <v>398</v>
       </c>
       <c r="C549">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D549" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="550" spans="1:4" x14ac:dyDescent="0.45">
@@ -28451,10 +28456,10 @@
         <v>398</v>
       </c>
       <c r="C550">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D550" t="s">
-        <v>1017</v>
+        <v>745</v>
       </c>
     </row>
     <row r="551" spans="1:4" x14ac:dyDescent="0.45">
@@ -28465,24 +28470,24 @@
         <v>398</v>
       </c>
       <c r="C551">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D551" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="552" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A552">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B552" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="C552">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="D552" t="s">
-        <v>970</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="553" spans="1:4" x14ac:dyDescent="0.45">
@@ -28493,10 +28498,10 @@
         <v>412</v>
       </c>
       <c r="C553">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D553" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="554" spans="1:4" x14ac:dyDescent="0.45">
@@ -28507,10 +28512,10 @@
         <v>412</v>
       </c>
       <c r="C554">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D554" t="s">
-        <v>885</v>
+        <v>971</v>
       </c>
     </row>
     <row r="555" spans="1:4" x14ac:dyDescent="0.45">
@@ -28521,10 +28526,10 @@
         <v>412</v>
       </c>
       <c r="C555">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D555" t="s">
-        <v>972</v>
+        <v>885</v>
       </c>
     </row>
     <row r="556" spans="1:4" x14ac:dyDescent="0.45">
@@ -28535,10 +28540,10 @@
         <v>412</v>
       </c>
       <c r="C556">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D556" t="s">
-        <v>1019</v>
+        <v>972</v>
       </c>
     </row>
     <row r="557" spans="1:4" x14ac:dyDescent="0.45">
@@ -28549,10 +28554,10 @@
         <v>412</v>
       </c>
       <c r="C557">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D557" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="558" spans="1:4" x14ac:dyDescent="0.45">
@@ -28563,24 +28568,24 @@
         <v>412</v>
       </c>
       <c r="C558">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D558" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="559" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A559">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B559" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C559">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D559" t="s">
-        <v>753</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="560" spans="1:4" x14ac:dyDescent="0.45">
@@ -28591,24 +28596,24 @@
         <v>415</v>
       </c>
       <c r="C560">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D560" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="561" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A561">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B561" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C561">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D561" t="s">
-        <v>784</v>
+        <v>754</v>
       </c>
     </row>
     <row r="562" spans="1:4" x14ac:dyDescent="0.45">
@@ -28619,10 +28624,10 @@
         <v>417</v>
       </c>
       <c r="C562">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D562" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="563" spans="1:4" x14ac:dyDescent="0.45">
@@ -28633,24 +28638,24 @@
         <v>417</v>
       </c>
       <c r="C563">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D563" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="564" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A564">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B564" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C564">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D564" t="s">
-        <v>750</v>
+        <v>786</v>
       </c>
     </row>
     <row r="565" spans="1:4" x14ac:dyDescent="0.45">
@@ -28661,10 +28666,10 @@
         <v>413</v>
       </c>
       <c r="C565">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D565" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="566" spans="1:4" x14ac:dyDescent="0.45">
@@ -28675,24 +28680,24 @@
         <v>413</v>
       </c>
       <c r="C566">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D566" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="567" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A567">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B567" t="s">
-        <v>21</v>
+        <v>413</v>
       </c>
       <c r="C567">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D567" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
     </row>
     <row r="568" spans="1:4" x14ac:dyDescent="0.45">
@@ -28703,10 +28708,10 @@
         <v>21</v>
       </c>
       <c r="C568">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D568" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="569" spans="1:4" x14ac:dyDescent="0.45">
@@ -28717,10 +28722,10 @@
         <v>21</v>
       </c>
       <c r="C569">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D569" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="570" spans="1:4" x14ac:dyDescent="0.45">
@@ -28731,10 +28736,10 @@
         <v>21</v>
       </c>
       <c r="C570">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D570" t="s">
-        <v>1022</v>
+        <v>757</v>
       </c>
     </row>
     <row r="571" spans="1:4" x14ac:dyDescent="0.45">
@@ -28745,10 +28750,10 @@
         <v>21</v>
       </c>
       <c r="C571">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D571" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="572" spans="1:4" x14ac:dyDescent="0.45">
@@ -28759,10 +28764,10 @@
         <v>21</v>
       </c>
       <c r="C572">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D572" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="573" spans="1:4" x14ac:dyDescent="0.45">
@@ -28773,10 +28778,10 @@
         <v>21</v>
       </c>
       <c r="C573">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D573" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="574" spans="1:4" x14ac:dyDescent="0.45">
@@ -28787,10 +28792,10 @@
         <v>21</v>
       </c>
       <c r="C574">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D574" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="575" spans="1:4" x14ac:dyDescent="0.45">
@@ -28801,10 +28806,10 @@
         <v>21</v>
       </c>
       <c r="C575">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D575" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="576" spans="1:4" x14ac:dyDescent="0.45">
@@ -28815,10 +28820,10 @@
         <v>21</v>
       </c>
       <c r="C576">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D576" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="577" spans="1:4" x14ac:dyDescent="0.45">
@@ -28829,10 +28834,10 @@
         <v>21</v>
       </c>
       <c r="C577">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D577" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="578" spans="1:4" x14ac:dyDescent="0.45">
@@ -28843,10 +28848,10 @@
         <v>21</v>
       </c>
       <c r="C578">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D578" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="579" spans="1:4" x14ac:dyDescent="0.45">
@@ -28857,10 +28862,10 @@
         <v>21</v>
       </c>
       <c r="C579">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D579" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="580" spans="1:4" x14ac:dyDescent="0.45">
@@ -28871,10 +28876,10 @@
         <v>21</v>
       </c>
       <c r="C580">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D580" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="581" spans="1:4" x14ac:dyDescent="0.45">
@@ -28885,10 +28890,10 @@
         <v>21</v>
       </c>
       <c r="C581">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D581" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="582" spans="1:4" x14ac:dyDescent="0.45">
@@ -28899,10 +28904,10 @@
         <v>21</v>
       </c>
       <c r="C582">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D582" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="583" spans="1:4" x14ac:dyDescent="0.45">
@@ -28913,10 +28918,10 @@
         <v>21</v>
       </c>
       <c r="C583">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D583" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="584" spans="1:4" x14ac:dyDescent="0.45">
@@ -28927,10 +28932,10 @@
         <v>21</v>
       </c>
       <c r="C584">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D584" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="585" spans="1:4" x14ac:dyDescent="0.45">
@@ -28941,10 +28946,10 @@
         <v>21</v>
       </c>
       <c r="C585">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D585" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="586" spans="1:4" x14ac:dyDescent="0.45">
@@ -28955,10 +28960,10 @@
         <v>21</v>
       </c>
       <c r="C586">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D586" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="587" spans="1:4" x14ac:dyDescent="0.45">
@@ -28969,10 +28974,10 @@
         <v>21</v>
       </c>
       <c r="C587">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D587" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="588" spans="1:4" x14ac:dyDescent="0.45">
@@ -28983,10 +28988,10 @@
         <v>21</v>
       </c>
       <c r="C588">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D588" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="589" spans="1:4" x14ac:dyDescent="0.45">
@@ -28997,10 +29002,10 @@
         <v>21</v>
       </c>
       <c r="C589">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D589" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="590" spans="1:4" x14ac:dyDescent="0.45">
@@ -29011,10 +29016,10 @@
         <v>21</v>
       </c>
       <c r="C590">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D590" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="591" spans="1:4" x14ac:dyDescent="0.45">
@@ -29025,10 +29030,10 @@
         <v>21</v>
       </c>
       <c r="C591">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D591" t="s">
-        <v>758</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="592" spans="1:4" x14ac:dyDescent="0.45">
@@ -29039,10 +29044,10 @@
         <v>21</v>
       </c>
       <c r="C592">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D592" t="s">
-        <v>1043</v>
+        <v>758</v>
       </c>
     </row>
     <row r="593" spans="1:4" x14ac:dyDescent="0.45">
@@ -29053,10 +29058,10 @@
         <v>21</v>
       </c>
       <c r="C593">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D593" t="s">
-        <v>759</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="594" spans="1:4" x14ac:dyDescent="0.45">
@@ -29067,10 +29072,10 @@
         <v>21</v>
       </c>
       <c r="C594">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D594" t="s">
-        <v>1044</v>
+        <v>759</v>
       </c>
     </row>
     <row r="595" spans="1:4" x14ac:dyDescent="0.45">
@@ -29081,10 +29086,10 @@
         <v>21</v>
       </c>
       <c r="C595">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D595" t="s">
-        <v>760</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="596" spans="1:4" x14ac:dyDescent="0.45">
@@ -29095,10 +29100,10 @@
         <v>21</v>
       </c>
       <c r="C596">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D596" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="597" spans="1:4" x14ac:dyDescent="0.45">
@@ -29109,10 +29114,10 @@
         <v>21</v>
       </c>
       <c r="C597">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D597" t="s">
-        <v>786</v>
+        <v>761</v>
       </c>
     </row>
     <row r="598" spans="1:4" x14ac:dyDescent="0.45">
@@ -29123,10 +29128,10 @@
         <v>21</v>
       </c>
       <c r="C598">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D598" t="s">
-        <v>762</v>
+        <v>786</v>
       </c>
     </row>
     <row r="599" spans="1:4" x14ac:dyDescent="0.45">
@@ -29137,10 +29142,10 @@
         <v>21</v>
       </c>
       <c r="C599">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D599" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="600" spans="1:4" x14ac:dyDescent="0.45">
@@ -29151,10 +29156,10 @@
         <v>21</v>
       </c>
       <c r="C600">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D600" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="601" spans="1:4" x14ac:dyDescent="0.45">
@@ -29165,10 +29170,10 @@
         <v>21</v>
       </c>
       <c r="C601">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D601" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="602" spans="1:4" x14ac:dyDescent="0.45">
@@ -29179,10 +29184,10 @@
         <v>21</v>
       </c>
       <c r="C602">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D602" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="603" spans="1:4" x14ac:dyDescent="0.45">
@@ -29193,10 +29198,10 @@
         <v>21</v>
       </c>
       <c r="C603">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D603" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="604" spans="1:4" x14ac:dyDescent="0.45">
@@ -29207,10 +29212,10 @@
         <v>21</v>
       </c>
       <c r="C604">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D604" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="605" spans="1:4" x14ac:dyDescent="0.45">
@@ -29221,10 +29226,10 @@
         <v>21</v>
       </c>
       <c r="C605">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D605" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="606" spans="1:4" x14ac:dyDescent="0.45">
@@ -29235,10 +29240,10 @@
         <v>21</v>
       </c>
       <c r="C606">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D606" t="s">
-        <v>1045</v>
+        <v>769</v>
       </c>
     </row>
     <row r="607" spans="1:4" x14ac:dyDescent="0.45">
@@ -29249,10 +29254,10 @@
         <v>21</v>
       </c>
       <c r="C607">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D607" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="608" spans="1:4" x14ac:dyDescent="0.45">
@@ -29263,10 +29268,10 @@
         <v>21</v>
       </c>
       <c r="C608">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D608" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="609" spans="1:4" x14ac:dyDescent="0.45">
@@ -29277,24 +29282,24 @@
         <v>21</v>
       </c>
       <c r="C609">
+        <v>45</v>
+      </c>
+      <c r="D609" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="610" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A610">
+        <v>38</v>
+      </c>
+      <c r="B610" t="s">
+        <v>21</v>
+      </c>
+      <c r="C610">
         <v>46</v>
       </c>
-      <c r="D609" t="s">
+      <c r="D610" t="s">
         <v>1048</v>
-      </c>
-    </row>
-    <row r="610" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A610" s="22">
-        <v>38</v>
-      </c>
-      <c r="B610" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C610" s="22">
-        <v>47</v>
-      </c>
-      <c r="D610" s="22" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="611" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
@@ -29305,24 +29310,24 @@
         <v>21</v>
       </c>
       <c r="C611" s="22">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D611" s="22" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="612" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A612" s="22">
         <v>38</v>
       </c>
-      <c r="B612" s="21" t="s">
+      <c r="B612" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C612" s="21">
-        <v>49</v>
-      </c>
-      <c r="D612" s="21" t="s">
-        <v>770</v>
+      <c r="C612" s="22">
+        <v>48</v>
+      </c>
+      <c r="D612" s="22" t="s">
+        <v>1050</v>
       </c>
     </row>
     <row r="613" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
@@ -29333,10 +29338,10 @@
         <v>21</v>
       </c>
       <c r="C613" s="21">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D613" s="21" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="614" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
@@ -29347,10 +29352,10 @@
         <v>21</v>
       </c>
       <c r="C614" s="21">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D614" s="21" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="615" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
@@ -29361,38 +29366,38 @@
         <v>21</v>
       </c>
       <c r="C615" s="21">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D615" s="21" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="616" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A616" s="22">
+        <v>38</v>
+      </c>
+      <c r="B616" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C616" s="21">
+        <v>52</v>
+      </c>
+      <c r="D616" s="21" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="617" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A617" s="22">
         <v>39</v>
       </c>
-      <c r="B616" s="22" t="s">
+      <c r="B617" s="22" t="s">
         <v>774</v>
       </c>
-      <c r="C616" s="22">
+      <c r="C617" s="22">
         <v>1</v>
       </c>
-      <c r="D616" s="22" t="s">
+      <c r="D617" s="22" t="s">
         <v>775</v>
-      </c>
-    </row>
-    <row r="617" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A617">
-        <v>39</v>
-      </c>
-      <c r="B617" t="s">
-        <v>774</v>
-      </c>
-      <c r="C617">
-        <v>3</v>
-      </c>
-      <c r="D617" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="618" spans="1:4" x14ac:dyDescent="0.45">
@@ -29403,24 +29408,24 @@
         <v>774</v>
       </c>
       <c r="C618">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D618" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="619" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A619">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B619" t="s">
-        <v>435</v>
+        <v>774</v>
       </c>
       <c r="C619">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D619" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="620" spans="1:4" x14ac:dyDescent="0.45">
@@ -29431,10 +29436,10 @@
         <v>435</v>
       </c>
       <c r="C620">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D620" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="621" spans="1:4" x14ac:dyDescent="0.45">
@@ -29445,24 +29450,24 @@
         <v>435</v>
       </c>
       <c r="C621">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D621" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="622" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A622">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B622" t="s">
-        <v>778</v>
+        <v>435</v>
       </c>
       <c r="C622">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D622" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
     </row>
     <row r="623" spans="1:4" x14ac:dyDescent="0.45">
@@ -29473,10 +29478,10 @@
         <v>778</v>
       </c>
       <c r="C623">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D623" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="624" spans="1:4" x14ac:dyDescent="0.45">
@@ -29487,24 +29492,24 @@
         <v>778</v>
       </c>
       <c r="C624">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D624" t="s">
-        <v>749</v>
+        <v>780</v>
       </c>
     </row>
     <row r="625" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A625">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B625" t="s">
-        <v>432</v>
+        <v>778</v>
       </c>
       <c r="C625">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D625" t="s">
-        <v>788</v>
+        <v>749</v>
       </c>
     </row>
     <row r="626" spans="1:4" x14ac:dyDescent="0.45">
@@ -29515,10 +29520,10 @@
         <v>432</v>
       </c>
       <c r="C626">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D626" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="627" spans="1:4" x14ac:dyDescent="0.45">
@@ -29529,10 +29534,10 @@
         <v>432</v>
       </c>
       <c r="C627">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D627" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="628" spans="1:4" x14ac:dyDescent="0.45">
@@ -29543,24 +29548,24 @@
         <v>432</v>
       </c>
       <c r="C628">
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="D628" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="629" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A629">
-        <v>43</v>
-      </c>
-      <c r="B629" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="C629" s="21">
-        <v>0</v>
-      </c>
-      <c r="D629" s="21" t="s">
-        <v>747</v>
+        <v>42</v>
+      </c>
+      <c r="B629" t="s">
+        <v>432</v>
+      </c>
+      <c r="C629">
+        <v>99</v>
+      </c>
+      <c r="D629" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="630" spans="1:4" x14ac:dyDescent="0.45">
@@ -29571,10 +29576,10 @@
         <v>152</v>
       </c>
       <c r="C630" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D630" s="21" t="s">
-        <v>1057</v>
+        <v>747</v>
       </c>
     </row>
     <row r="631" spans="1:4" x14ac:dyDescent="0.45">
@@ -29585,10 +29590,10 @@
         <v>152</v>
       </c>
       <c r="C631" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D631" s="21" t="s">
-        <v>1066</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="632" spans="1:4" x14ac:dyDescent="0.45">
@@ -29599,24 +29604,24 @@
         <v>152</v>
       </c>
       <c r="C632" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D632" s="21" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="633" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A633">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B633" s="21" t="s">
-        <v>1134</v>
+        <v>152</v>
       </c>
       <c r="C633" s="21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D633" s="21" t="s">
-        <v>747</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="634" spans="1:4" x14ac:dyDescent="0.45">
@@ -29627,38 +29632,38 @@
         <v>1134</v>
       </c>
       <c r="C634" s="21">
+        <v>0</v>
+      </c>
+      <c r="D634" s="21" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="635" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A635">
+        <v>44</v>
+      </c>
+      <c r="B635" s="21" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C635" s="21">
         <v>1</v>
       </c>
-      <c r="D634" s="21" t="s">
+      <c r="D635" s="21" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="635" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A635" s="45">
+    <row r="636" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A636" s="45">
         <v>44</v>
       </c>
-      <c r="B635" s="45" t="s">
+      <c r="B636" s="45" t="s">
         <v>1134</v>
       </c>
-      <c r="C635" s="45">
+      <c r="C636" s="45">
         <v>-1</v>
       </c>
-      <c r="D635" s="45" t="s">
+      <c r="D636" s="45" t="s">
         <v>786</v>
-      </c>
-    </row>
-    <row r="636" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A636">
-        <v>45</v>
-      </c>
-      <c r="B636" s="21" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C636" s="21">
-        <v>0</v>
-      </c>
-      <c r="D636" s="21" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="637" spans="1:4" x14ac:dyDescent="0.45">
@@ -29669,10 +29674,10 @@
         <v>1136</v>
       </c>
       <c r="C637" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D637" s="21" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="638" spans="1:4" x14ac:dyDescent="0.45">
@@ -29683,24 +29688,24 @@
         <v>1136</v>
       </c>
       <c r="C638" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D638" s="21" t="s">
-        <v>1137</v>
+        <v>748</v>
       </c>
     </row>
     <row r="639" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A639">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B639" s="21" t="s">
-        <v>281</v>
+        <v>1136</v>
       </c>
       <c r="C639" s="21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D639" s="21" t="s">
-        <v>1160</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="640" spans="1:4" x14ac:dyDescent="0.45">
@@ -29711,10 +29716,10 @@
         <v>281</v>
       </c>
       <c r="C640" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D640" s="21" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="641" spans="1:4" x14ac:dyDescent="0.45">
@@ -29725,14 +29730,28 @@
         <v>281</v>
       </c>
       <c r="C641" s="21">
+        <v>1</v>
+      </c>
+      <c r="D641" s="21" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="642" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A642">
+        <v>46</v>
+      </c>
+      <c r="B642" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="C642" s="21">
         <v>99</v>
       </c>
-      <c r="D641" s="21" t="s">
+      <c r="D642" s="21" t="s">
         <v>875</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D632" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:D633" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -29743,7 +29762,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H76" sqref="H76"/>
     </sheetView>

</xml_diff>